<commit_message>
MPTrx - updated to work without specializations (to circumvent issue #628 (or was it #625?)
</commit_message>
<xml_diff>
--- a/MPTrx/Car Insurance Case.xlsx
+++ b/MPTrx/Car Insurance Case.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="13800" windowHeight="5472" tabRatio="703" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="13800" windowHeight="5472" tabRatio="703" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="#Scopes" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="97">
   <si>
     <t>Customer</t>
   </si>
@@ -226,9 +226,6 @@
     <t>Price of car [licenseplate], according to the catalogue of the manufacturer, in Euro.</t>
   </si>
   <si>
-    <t>TParty</t>
-  </si>
-  <si>
     <t>[TParties]</t>
   </si>
   <si>
@@ -241,9 +238,6 @@
     <t>[Concerns]</t>
   </si>
   <si>
-    <t>Concern</t>
-  </si>
-  <si>
     <t>Beslissing</t>
   </si>
   <si>
@@ -298,9 +292,6 @@
     <t>mptrxIsaCasus</t>
   </si>
   <si>
-    <t>MPTrx</t>
-  </si>
-  <si>
     <t>AttrProvider</t>
   </si>
   <si>
@@ -311,6 +302,12 @@
   </si>
   <si>
     <t>ttDescr</t>
+  </si>
+  <si>
+    <t>ttIsaTParty</t>
+  </si>
+  <si>
+    <t>ttIsaConcern</t>
   </si>
 </sst>
 </file>
@@ -759,7 +756,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,15 +780,15 @@
         <v>33</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>35</v>
@@ -802,8 +799,9 @@
       <c r="D2" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="20" t="s">
-        <v>93</v>
+      <c r="E2" s="20" t="str">
+        <f>$A2</f>
+        <v>Scope</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -834,222 +832,265 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="14" customWidth="1"/>
-    <col min="4" max="4" width="64.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" style="23" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="14" customWidth="1"/>
+    <col min="1" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="14" customWidth="1"/>
+    <col min="5" max="5" width="64.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="23" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="str">
+        <f>IF($A2="","",$A2)</f>
+        <v>TText</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="str">
-        <f>IF(OR($B3="",$C3=""),"",CONCATENATE("SHR_",$B3,"_",$C3))</f>
+        <f>IF(OR($C3="",$D3=""),"",CONCATENATE("SHR_",$C3,"_",$D3))</f>
         <v>SHR_MPTrx1v0.1_12-AB-34_Insurer</v>
       </c>
-      <c r="B3" s="21" t="str">
-        <f>IF($C3="","",'#Scopes'!$A$3)</f>
-        <v>MPTrx1v0.1_12-AB-34</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="4" t="str">
+        <f>IF($A3="","",$A3)</f>
+        <v>SHR_MPTrx1v0.1_12-AB-34_Insurer</v>
+      </c>
+      <c r="C3" s="21" t="str">
+        <f>IF($D3="","",'#Scopes'!$A$3)</f>
+        <v>MPTrx1v0.1_12-AB-34</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="E3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="str">
-        <f t="shared" ref="A4:A11" si="0">IF(OR($B4="",$C4=""),"",CONCATENATE("SHR_",$B4,"_",$C4))</f>
+        <f t="shared" ref="A4:A11" si="0">IF(OR($C4="",$D4=""),"",CONCATENATE("SHR_",$C4,"_",$D4))</f>
         <v>SHR_MPTrx1v0.1_12-AB-34_RDW</v>
       </c>
-      <c r="B4" s="21" t="str">
-        <f>IF($C4="","",'#Scopes'!$A$3)</f>
-        <v>MPTrx1v0.1_12-AB-34</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="4" t="str">
+        <f t="shared" ref="B4:B11" si="1">IF($A4="","",$A4)</f>
+        <v>SHR_MPTrx1v0.1_12-AB-34_RDW</v>
+      </c>
+      <c r="C4" s="21" t="str">
+        <f>IF($D4="","",'#Scopes'!$A$3)</f>
+        <v>MPTrx1v0.1_12-AB-34</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="E4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="G4" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>SHR_MPTrx1v0.1_12-AB-34_AttrProvider</v>
       </c>
-      <c r="B5" s="21" t="str">
-        <f>IF($C5="","",'#Scopes'!$A$3)</f>
-        <v>MPTrx1v0.1_12-AB-34</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="B5" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>SHR_MPTrx1v0.1_12-AB-34_AttrProvider</v>
+      </c>
+      <c r="C5" s="21" t="str">
+        <f>IF($D5="","",'#Scopes'!$A$3)</f>
+        <v>MPTrx1v0.1_12-AB-34</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="str">
-        <f>IF(OR($B6="",$C6=""),"",CONCATENATE("SHR_",$B6,"_",$C6))</f>
+        <f>IF(OR($C6="",$D6=""),"",CONCATENATE("SHR_",$C6,"_",$D6))</f>
         <v>SHR_MPTrx1v0.1_12-AB-34_Customer</v>
       </c>
-      <c r="B6" s="21" t="str">
-        <f>IF($C6="","",'#Scopes'!$A$3)</f>
-        <v>MPTrx1v0.1_12-AB-34</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>SHR_MPTrx1v0.1_12-AB-34_Customer</v>
+      </c>
+      <c r="C6" s="21" t="str">
+        <f>IF($D6="","",'#Scopes'!$A$3)</f>
+        <v>MPTrx1v0.1_12-AB-34</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>SHR_MPTrx1v0.1_12-AB-34_Driver</v>
       </c>
-      <c r="B7" s="21" t="str">
-        <f>IF($C7="","",'#Scopes'!$A$3)</f>
-        <v>MPTrx1v0.1_12-AB-34</v>
-      </c>
-      <c r="C7" s="14" t="s">
+      <c r="B7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>SHR_MPTrx1v0.1_12-AB-34_Driver</v>
+      </c>
+      <c r="C7" s="21" t="str">
+        <f>IF($D7="","",'#Scopes'!$A$3)</f>
+        <v>MPTrx1v0.1_12-AB-34</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="E7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="G7" s="14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>SHR_MPTrx1v0.1_12-AB-34_PrevInsurer</v>
       </c>
-      <c r="B8" s="21" t="str">
-        <f>IF($C8="","",'#Scopes'!$A$3)</f>
-        <v>MPTrx1v0.1_12-AB-34</v>
-      </c>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>SHR_MPTrx1v0.1_12-AB-34_PrevInsurer</v>
+      </c>
+      <c r="C8" s="21" t="str">
+        <f>IF($D8="","",'#Scopes'!$A$3)</f>
+        <v>MPTrx1v0.1_12-AB-34</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="E8" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>SHR_MPTrx1v0.1_12-AB-34_Computer</v>
       </c>
-      <c r="B9" s="21" t="str">
-        <f>IF($C9="","",'#Scopes'!$A$3)</f>
-        <v>MPTrx1v0.1_12-AB-34</v>
-      </c>
-      <c r="C9" s="14" t="s">
+      <c r="B9" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>SHR_MPTrx1v0.1_12-AB-34_Computer</v>
+      </c>
+      <c r="C9" s="21" t="str">
+        <f>IF($D9="","",'#Scopes'!$A$3)</f>
+        <v>MPTrx1v0.1_12-AB-34</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="E9" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B10" s="21" t="str">
-        <f>IF($C10="","",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="18"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C10" s="21" t="str">
+        <f>IF($D10="","",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="18"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B11" s="21" t="str">
-        <f>IF($C11="","",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="8"/>
+      <c r="B11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C11" s="21" t="str">
+        <f>IF($D11="","",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1058,241 +1099,312 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="14" customWidth="1"/>
-    <col min="5" max="5" width="86.6640625" customWidth="1"/>
+    <col min="1" max="2" width="43.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="86.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="25" t="str">
+        <f>IF($A2="","",$A2)</f>
+        <v>TText</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>41</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="str">
-        <f>IF(OR($B3="",$C3=""),"",CONCATENATE("Conc_",$B3,"_",$C3))</f>
+        <f>IF(OR($C3="",$D3=""),"",CONCATENATE("Conc_",$C3,"_",$D3))</f>
         <v>Conc_MPTrx1v0.1_12-AB-34_Beslissing</v>
       </c>
-      <c r="B3" s="15" t="str">
-        <f>IF(AND($E3="",$C3=""),"",'#Scopes'!$A$3)</f>
-        <v>MPTrx1v0.1_12-AB-34</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="B3" s="17" t="str">
+        <f t="shared" ref="B3:B18" si="0">IF($A3="","",$A3)</f>
+        <v>Conc_MPTrx1v0.1_12-AB-34_Beslissing</v>
+      </c>
+      <c r="C3" s="15" t="str">
+        <f>IF(AND($F3="",$D3=""),"",'#Scopes'!$A$3)</f>
+        <v>MPTrx1v0.1_12-AB-34</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="str">
+        <f t="shared" ref="A4:A18" si="1">IF(OR($C4="",$D4=""),"",CONCATENATE("Conc_",$C4,"_",$D4))</f>
+        <v>Conc_MPTrx1v0.1_12-AB-34_Customer Agreement</v>
+      </c>
+      <c r="B4" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Conc_MPTrx1v0.1_12-AB-34_Customer Agreement</v>
+      </c>
+      <c r="C4" s="15" t="str">
+        <f>IF(AND($F4="",$D4=""),"",'#Scopes'!$A$3)</f>
+        <v>MPTrx1v0.1_12-AB-34</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Conc_MPTrx1v0.1_12-AB-34_Eigen Risico</v>
+      </c>
+      <c r="B5" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Conc_MPTrx1v0.1_12-AB-34_Eigen Risico</v>
+      </c>
+      <c r="C5" s="15" t="str">
+        <f>IF(AND($F5="",$D5=""),"",'#Scopes'!$A$3)</f>
+        <v>MPTrx1v0.1_12-AB-34</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="str">
-        <f t="shared" ref="A4:A18" si="0">IF(OR($B4="",$C4=""),"",CONCATENATE("Conc_",$B4,"_",$C4))</f>
-        <v>Conc_MPTrx1v0.1_12-AB-34_Customer Agreement</v>
-      </c>
-      <c r="B4" s="15" t="str">
-        <f>IF(AND($E4="",$C4=""),"",'#Scopes'!$A$3)</f>
-        <v>MPTrx1v0.1_12-AB-34</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="E5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>Conc_MPTrx1v0.1_12-AB-34_Eigen Risico</v>
-      </c>
-      <c r="B5" s="15" t="str">
-        <f>IF(AND($E5="",$C5=""),"",'#Scopes'!$A$3)</f>
-        <v>MPTrx1v0.1_12-AB-34</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B6" s="15" t="str">
-        <f>IF(AND($E6="",$C6=""),"",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B6" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C6" s="15" t="str">
+        <f>IF(AND($F6="",$D6=""),"",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B7" s="15" t="str">
-        <f>IF(AND($E7="",$C7=""),"",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B7" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C7" s="15" t="str">
+        <f>IF(AND($F7="",$D7=""),"",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B8" s="15" t="str">
-        <f>IF(AND($E8="",$C8=""),"",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B8" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C8" s="15" t="str">
+        <f>IF(AND($F8="",$D8=""),"",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B9" s="15" t="str">
-        <f>IF(AND($E9="",$C9=""),"",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B9" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C9" s="15" t="str">
+        <f>IF(AND($F9="",$D9=""),"",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B10" s="15" t="str">
-        <f>IF(AND($E10="",$C10=""),"",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B10" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C10" s="15" t="str">
+        <f>IF(AND($F10="",$D10=""),"",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B11" s="15" t="str">
-        <f>IF(AND($E11="",$C11=""),"",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B11" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C11" s="15" t="str">
+        <f>IF(AND($F11="",$D11=""),"",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B12" s="15" t="str">
-        <f>IF(AND($E12="",$C12=""),"",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B12" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C12" s="15" t="str">
+        <f>IF(AND($F12="",$D12=""),"",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B13" s="15" t="str">
-        <f>IF(AND($E13="",$C13=""),"",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B13" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C13" s="15" t="str">
+        <f>IF(AND($F13="",$D13=""),"",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B14" s="15" t="str">
-        <f>IF(AND($E14="",$C14=""),"",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B14" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C14" s="15" t="str">
+        <f>IF(AND($F14="",$D14=""),"",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B15" s="15" t="str">
-        <f>IF(AND($E15="",$C15=""),"",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B15" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C15" s="15" t="str">
+        <f>IF(AND($F15="",$D15=""),"",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B16" s="15" t="str">
-        <f>IF(AND($E16="",$C16=""),"",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B16" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C16" s="15" t="str">
+        <f>IF(AND($F16="",$D16=""),"",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B17" s="15" t="str">
-        <f>IF(AND($E17="",$C17=""),"",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B17" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C17" s="15" t="str">
+        <f>IF(AND($F17="",$D17=""),"",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B18" s="15" t="str">
-        <f>IF(AND($E18="",$C18=""),"",'#Scopes'!$A$3)</f>
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B18" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C18" s="15" t="str">
+        <f>IF(AND($F18="",$D18=""),"",'#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -1413,7 +1525,7 @@
         <v>63</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>0</v>
@@ -1422,7 +1534,7 @@
         <v>60</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -1469,7 +1581,7 @@
         <v>59</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
@@ -1488,7 +1600,7 @@
         <v>5094</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>58</v>
@@ -1510,7 +1622,7 @@
         <v>46</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>57</v>
@@ -1534,7 +1646,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>62</v>
@@ -1560,7 +1672,7 @@
         <v>55</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
@@ -1582,7 +1694,7 @@
         <v>56</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
@@ -1724,13 +1836,13 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1743,13 +1855,13 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1762,13 +1874,13 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1781,13 +1893,13 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
MPTrx - major update. It starts to work nicely now.
</commit_message>
<xml_diff>
--- a/MPTrx/Car Insurance Case.xlsx
+++ b/MPTrx/Car Insurance Case.xlsx
@@ -235,9 +235,6 @@
     <t>tPartyReqdOrg</t>
   </si>
   <si>
-    <t>[Concerns]</t>
-  </si>
-  <si>
     <t>Beslissing</t>
   </si>
   <si>
@@ -307,7 +304,10 @@
     <t>ttIsaTParty</t>
   </si>
   <si>
-    <t>ttIsaConcern</t>
+    <t>[Objectives]</t>
+  </si>
+  <si>
+    <t>ttIsaObjective</t>
   </si>
 </sst>
 </file>
@@ -780,10 +780,10 @@
         <v>33</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -853,7 +853,7 @@
         <v>69</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>37</v>
@@ -862,7 +862,7 @@
         <v>38</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>71</v>
@@ -961,7 +961,7 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>13</v>
@@ -1102,12 +1102,13 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="43.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.77734375" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="19.77734375" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.44140625" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.109375" style="14" customWidth="1"/>
@@ -1116,7 +1117,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>96</v>
@@ -1157,71 +1158,71 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="str">
-        <f>IF(OR($C3="",$D3=""),"",CONCATENATE("Conc_",$C3,"_",$D3))</f>
-        <v>Conc_MPTrx1v0.1_12-AB-34_Beslissing</v>
+        <f>IF(OR($C3="",$D3=""),"",CONCATENATE("Obj_",$C3,"_",$D3))</f>
+        <v>Obj_MPTrx1v0.1_12-AB-34_Beslissing</v>
       </c>
       <c r="B3" s="17" t="str">
-        <f t="shared" ref="B3:B18" si="0">IF($A3="","",$A3)</f>
-        <v>Conc_MPTrx1v0.1_12-AB-34_Beslissing</v>
+        <f t="shared" ref="B3" si="0">IF($A3="","",$A3)</f>
+        <v>Obj_MPTrx1v0.1_12-AB-34_Beslissing</v>
       </c>
       <c r="C3" s="15" t="str">
         <f>IF(AND($F3="",$D3=""),"",'#Scopes'!$A$3)</f>
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="str">
-        <f t="shared" ref="A4:A18" si="1">IF(OR($C4="",$D4=""),"",CONCATENATE("Conc_",$C4,"_",$D4))</f>
-        <v>Conc_MPTrx1v0.1_12-AB-34_Customer Agreement</v>
+        <f t="shared" ref="A4:A18" si="1">IF(OR($C4="",$D4=""),"",CONCATENATE("Obj_",$C4,"_",$D4))</f>
+        <v>Obj_MPTrx1v0.1_12-AB-34_Customer Agreement</v>
       </c>
       <c r="B4" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>Conc_MPTrx1v0.1_12-AB-34_Customer Agreement</v>
+        <f t="shared" ref="B4:B18" si="2">IF($A4="","",$A4)</f>
+        <v>Obj_MPTrx1v0.1_12-AB-34_Customer Agreement</v>
       </c>
       <c r="C4" s="15" t="str">
         <f>IF(AND($F4="",$D4=""),"",'#Scopes'!$A$3)</f>
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>Conc_MPTrx1v0.1_12-AB-34_Eigen Risico</v>
+        <v>Obj_MPTrx1v0.1_12-AB-34_Eigen Risico</v>
       </c>
       <c r="B5" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>Conc_MPTrx1v0.1_12-AB-34_Eigen Risico</v>
+        <f t="shared" si="2"/>
+        <v>Obj_MPTrx1v0.1_12-AB-34_Eigen Risico</v>
       </c>
       <c r="C5" s="15" t="str">
         <f>IF(AND($F5="",$D5=""),"",'#Scopes'!$A$3)</f>
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1230,7 +1231,7 @@
         <v/>
       </c>
       <c r="B6" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C6" s="15" t="str">
@@ -1245,7 +1246,7 @@
         <v/>
       </c>
       <c r="B7" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C7" s="15" t="str">
@@ -1260,7 +1261,7 @@
         <v/>
       </c>
       <c r="B8" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C8" s="15" t="str">
@@ -1274,7 +1275,7 @@
         <v/>
       </c>
       <c r="B9" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C9" s="15" t="str">
@@ -1288,7 +1289,7 @@
         <v/>
       </c>
       <c r="B10" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C10" s="15" t="str">
@@ -1302,7 +1303,7 @@
         <v/>
       </c>
       <c r="B11" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C11" s="15" t="str">
@@ -1316,7 +1317,7 @@
         <v/>
       </c>
       <c r="B12" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C12" s="15" t="str">
@@ -1330,7 +1331,7 @@
         <v/>
       </c>
       <c r="B13" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C13" s="15" t="str">
@@ -1344,7 +1345,7 @@
         <v/>
       </c>
       <c r="B14" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C14" s="15" t="str">
@@ -1358,7 +1359,7 @@
         <v/>
       </c>
       <c r="B15" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C15" s="15" t="str">
@@ -1372,7 +1373,7 @@
         <v/>
       </c>
       <c r="B16" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C16" s="15" t="str">
@@ -1386,7 +1387,7 @@
         <v/>
       </c>
       <c r="B17" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C17" s="15" t="str">
@@ -1400,7 +1401,7 @@
         <v/>
       </c>
       <c r="B18" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C18" s="15" t="str">
@@ -1525,7 +1526,7 @@
         <v>63</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>0</v>
@@ -1534,7 +1535,7 @@
         <v>60</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -1581,7 +1582,7 @@
         <v>59</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
@@ -1600,7 +1601,7 @@
         <v>5094</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>58</v>
@@ -1622,7 +1623,7 @@
         <v>46</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>57</v>
@@ -1646,7 +1647,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>62</v>
@@ -1672,7 +1673,7 @@
         <v>55</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
@@ -1694,7 +1695,7 @@
         <v>56</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
@@ -1836,13 +1837,13 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1855,13 +1856,13 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1874,13 +1875,13 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1893,13 +1894,13 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
MPTrx - revised for revised SIAMv3, and refactoring bugfixes
</commit_message>
<xml_diff>
--- a/MPTrx/Car Insurance Case.xlsx
+++ b/MPTrx/Car Insurance Case.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="13800" windowHeight="5472" tabRatio="703" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="13800" windowHeight="5472" tabRatio="703" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="#Scopes" sheetId="1" r:id="rId1"/>
@@ -148,9 +148,6 @@
     <t>TTPhrase</t>
   </si>
   <si>
-    <t>[Organization,]</t>
-  </si>
-  <si>
     <t>ttValue</t>
   </si>
   <si>
@@ -232,9 +229,6 @@
     <t>tPartyAcc</t>
   </si>
   <si>
-    <t>tPartyReqdOrg</t>
-  </si>
-  <si>
     <t>Beslissing</t>
   </si>
   <si>
@@ -308,6 +302,12 @@
   </si>
   <si>
     <t>ttIsaObjective</t>
+  </si>
+  <si>
+    <t>tPartyReqdOrgRef</t>
+  </si>
+  <si>
+    <t>OrgRef</t>
   </si>
 </sst>
 </file>
@@ -376,7 +376,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -436,12 +436,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -779,11 +773,11 @@
       <c r="C1" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" s="24" t="s">
+      <c r="D1" s="22" t="s">
         <v>89</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -796,7 +790,7 @@
       <c r="C2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="22" t="s">
         <v>41</v>
       </c>
       <c r="E2" s="20" t="str">
@@ -817,7 +811,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" s="8" t="str">
         <f>$A3</f>
@@ -834,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -844,16 +838,16 @@
     <col min="3" max="3" width="19.77734375" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="14" customWidth="1"/>
     <col min="5" max="5" width="64.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="23" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="14" customWidth="1"/>
     <col min="7" max="7" width="10.44140625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>37</v>
@@ -862,13 +856,13 @@
         <v>38</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>71</v>
+        <v>91</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -879,7 +873,7 @@
         <f>IF($A2="","",$A2)</f>
         <v>TText</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
@@ -888,11 +882,11 @@
       <c r="E2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>43</v>
+      <c r="F2" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -914,11 +908,11 @@
       <c r="E3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -940,11 +934,11 @@
       <c r="E4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -961,14 +955,14 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="22"/>
+      <c r="F5" s="8"/>
       <c r="G5" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -990,9 +984,9 @@
       <c r="E6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1015,7 +1009,7 @@
         <v>18</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1089,7 +1083,7 @@
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="18"/>
-      <c r="F11" s="10"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="8"/>
     </row>
   </sheetData>
@@ -1101,7 +1095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -1115,12 +1109,12 @@
     <col min="6" max="6" width="86.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>96</v>
+    <row r="1" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>94</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>37</v>
@@ -1135,11 +1129,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="25" t="str">
+      <c r="B2" s="23" t="str">
         <f>IF($A2="","",$A2)</f>
         <v>TText</v>
       </c>
@@ -1170,13 +1164,13 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1193,13 +1187,13 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1216,13 +1210,13 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1448,7 +1442,7 @@
         <v>38</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>39</v>
@@ -1486,7 +1480,7 @@
         <v>41</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>41</v>
@@ -1523,19 +1517,19 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -1556,7 +1550,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K4" s="7"/>
     </row>
@@ -1579,10 +1573,10 @@
         <v>14</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
@@ -1597,14 +1591,14 @@
       <c r="C6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="24">
         <v>5094</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
@@ -1620,13 +1614,13 @@
         <v>8</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -1647,10 +1641,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M8" s="7"/>
     </row>
@@ -1670,10 +1664,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
@@ -1692,10 +1686,10 @@
         <v>6</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
@@ -1730,13 +1724,13 @@
         <v>25</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
@@ -1752,13 +1746,13 @@
         <v>26</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
@@ -1780,7 +1774,7 @@
         <v>6</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
@@ -1802,7 +1796,7 @@
         <v>6</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
@@ -1824,7 +1818,7 @@
         <v>6</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1837,13 +1831,13 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1856,13 +1850,13 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1875,13 +1869,13 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1894,13 +1888,13 @@
         <v>MPTrx1v0.1_12-AB-34</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>